<commit_message>
PLC Handler PLC Simulator
</commit_message>
<xml_diff>
--- a/Warehouse Manager/Database/Orders.xlsx
+++ b/Warehouse Manager/Database/Orders.xlsx
@@ -475,7 +475,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>50001</v>
+        <v>50006</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -483,25 +483,25 @@
         </is>
       </c>
       <c r="C2" s="5" t="n">
-        <v>45071.8710108066</v>
+        <v>45072.29391293159</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>45071.8710108066</v>
+        <v>45072.29391293159</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Supplier Z</t>
+          <t>Supplier J</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[{'Name': 'Power Drill', 'Quantity': 100}, {'Name': 'Paint Brush Set', 'Quantity': 200}]</t>
+          <t>[{'Name': 'Meditation Cushion', 'Quantity': 100}, {'Name': 'Yoga Mat', 'Quantity': 300}]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>50002</v>
+        <v>50007</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -509,25 +509,25 @@
         </is>
       </c>
       <c r="C3" s="5" t="n">
-        <v>45071.87101085933</v>
+        <v>45072.29391294316</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>45071.87101085933</v>
+        <v>45072.29391294316</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Supplier C</t>
+          <t>Supplier Q</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[{'Name': 'Bluetooth Speaker', 'Quantity': 200}, {'Name': 'Wireless Headphones', 'Quantity': 300}, {'Name': 'Wireless Mouse', 'Quantity': 200}]</t>
+          <t>[{'Name': 'Steam Iron', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>50003</v>
+        <v>50011</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -535,25 +535,25 @@
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>45071.87101091742</v>
+        <v>45072.29391297736</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>45071.87102249149</v>
+        <v>45072.29392455144</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Supplier M</t>
+          <t>Supplier D</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[{'Name': 'Eyeshadow Palette', 'Quantity': 500}, {'Name': 'Mascara', 'Quantity': 500}]</t>
+          <t>[{'Name': 'Laptop Backpack', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>50005</v>
+        <v>50016</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -561,25 +561,25 @@
         </is>
       </c>
       <c r="C5" s="5" t="n">
-        <v>45071.87101100563</v>
+        <v>45072.29391304119</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>45071.8710225797</v>
+        <v>45072.29392461527</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Supplier B</t>
+          <t>Supplier R</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[{'Name': 'USB Flash Drive', 'Quantity': 500}, {'Name': 'HDMI Cable', 'Quantity': 200}]</t>
+          <t>[{'Name': 'Vacuum Cleaner', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>50007</v>
+        <v>50015</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -587,25 +587,25 @@
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>45071.87101107732</v>
+        <v>45072.29391304119</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>45071.87101107732</v>
+        <v>45072.29391304119</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Supplier E</t>
+          <t>Supplier L</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[{'Name': 'LED Bulb', 'Quantity': 1000}, {'Name': 'Floor Lamp', 'Quantity': 100}]</t>
+          <t>[{'Name': 'Facial Cleanser', 'Quantity': 500}]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>50011</v>
+        <v>50018</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -613,25 +613,25 @@
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>45071.87101129258</v>
+        <v>45072.29391307591</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>45071.87101129258</v>
+        <v>45072.29392464999</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Supplier J</t>
+          <t>Supplier S</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[{'Name': 'Yoga Mat', 'Quantity': 300}, {'Name': 'Yoga Block', 'Quantity': 100}, {'Name': 'Resistance Bands', 'Quantity': 500}]</t>
+          <t>[{'Name': 'Knife Set', 'Quantity': 100}, {'Name': 'Mixing Bowl Set', 'Quantity': 200}, {'Name': 'Cutting Board', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>50012</v>
+        <v>50020</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -639,25 +639,25 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>45071.87101132313</v>
+        <v>45072.29391310572</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>45071.87101132313</v>
+        <v>45072.29391310572</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Supplier O</t>
+          <t>Supplier A</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[{'Name': 'Bath Towels', 'Quantity': 400}]</t>
+          <t>[{'Name': 'AAA Batteries', 'Quantity': 1000}]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>50013</v>
+        <v>50001</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -665,25 +665,25 @@
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>45071.87101135292</v>
+        <v>45072.2939243917</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>45071.87101135292</v>
+        <v>45072.2939243917</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Supplier L</t>
+          <t>Supplier Z</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[{'Name': 'Facial Cleanser', 'Quantity': 500}]</t>
+          <t>[{'Name': 'Power Drill', 'Quantity': 100}, {'Name': 'Paint Roller Kit', 'Quantity': 100}, {'Name': 'Paint Brush Set', 'Quantity': 200}]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>50015</v>
+        <v>50002</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -691,25 +691,25 @@
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>45071.87101151001</v>
+        <v>45072.29392440324</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>45071.87101151001</v>
+        <v>45072.29393597732</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Supplier K</t>
+          <t>Supplier R</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[{'Name': 'Aromatherapy Diffuser', 'Quantity': 500}]</t>
+          <t>[{'Name': 'Vacuum Cleaner', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>50018</v>
+        <v>50003</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -717,25 +717,25 @@
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>45071.87101158587</v>
+        <v>45072.29392444387</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>45071.87101158587</v>
+        <v>45072.29392444387</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Supplier O</t>
+          <t>Supplier Y</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[{'Name': 'Bath Towels', 'Quantity': 400}]</t>
+          <t>[{'Name': 'Screw Assortment Kit', 'Quantity': 500}, {'Name': 'Toolbox', 'Quantity': 100}, {'Name': 'Level', 'Quantity': 200}, {'Name': 'Utility Knife', 'Quantity': 200}]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>50020</v>
+        <v>50004</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>45071.87101169641</v>
+        <v>45072.29392447034</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>45071.87102327048</v>
+        <v>45072.29392447034</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -755,13 +755,13 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[{'Name': 'Meditation Cushion', 'Quantity': 100}, {'Name': 'Yoga Mat', 'Quantity': 300}, {'Name': 'Yoga Block', 'Quantity': 100}, {'Name': 'Resistance Bands', 'Quantity': 500}]</t>
+          <t>[{'Name': 'Meditation Cushion', 'Quantity': 100}, {'Name': 'Yoga Mat', 'Quantity': 300}, {'Name': 'Yoga Block', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>50004</v>
+        <v>50005</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -769,25 +769,25 @@
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>45071.87102254497</v>
+        <v>45072.29392448255</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>45071.87103411904</v>
+        <v>45072.29393605662</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Supplier C</t>
+          <t>Supplier W</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[{'Name': 'Bluetooth Speaker', 'Quantity': 200}, {'Name': 'Wireless Headphones', 'Quantity': 300}, {'Name': 'Wireless Mouse', 'Quantity': 200}]</t>
+          <t>[{'Name': 'Blender', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>50006</v>
+        <v>50009</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -795,19 +795,19 @@
         </is>
       </c>
       <c r="C14" s="5" t="n">
-        <v>45071.87102260287</v>
+        <v>45072.29392452884</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>45071.87102260287</v>
+        <v>45072.29392452884</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Supplier L</t>
+          <t>Supplier W</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[{'Name': 'Moisturizing Cream', 'Quantity': 300}]</t>
+          <t>[{'Name': 'Blender', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
@@ -821,25 +821,25 @@
         </is>
       </c>
       <c r="C15" s="5" t="n">
-        <v>45071.87102269609</v>
+        <v>45072.29392452884</v>
       </c>
       <c r="D15" s="5" t="n">
-        <v>45071.87102269609</v>
+        <v>45072.29392452884</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Supplier S</t>
+          <t>Supplier O</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[{'Name': 'Cutting Board', 'Quantity': 100}, {'Name': 'Mixing Bowl Set', 'Quantity': 200}]</t>
+          <t>[{'Name': 'Bed Sheets', 'Quantity': 200}]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>50009</v>
+        <v>50010</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -847,25 +847,25 @@
         </is>
       </c>
       <c r="C16" s="5" t="n">
-        <v>45071.8710227436</v>
+        <v>45072.29392454039</v>
       </c>
       <c r="D16" s="5" t="n">
-        <v>45071.8710227436</v>
+        <v>45072.29393611447</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Supplier M</t>
+          <t>Supplier R</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[{'Name': 'Eyeshadow Palette', 'Quantity': 500}, {'Name': 'Mascara', 'Quantity': 500}, {'Name': 'Lipstick', 'Quantity': 500}]</t>
+          <t>[{'Name': 'Vacuum Cleaner', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>50010</v>
+        <v>50012</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -873,25 +873,25 @@
         </is>
       </c>
       <c r="C17" s="5" t="n">
-        <v>45071.87102279678</v>
+        <v>45072.29392456885</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>45071.87102279678</v>
+        <v>45072.29392456885</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Supplier M</t>
+          <t>Supplier L</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[{'Name': 'Eyeshadow Palette', 'Quantity': 500}, {'Name': 'Mascara', 'Quantity': 500}, {'Name': 'Lipstick', 'Quantity': 500}]</t>
+          <t>[{'Name': 'Moisturizing Cream', 'Quantity': 300}]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>50014</v>
+        <v>50013</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -899,25 +899,25 @@
         </is>
       </c>
       <c r="C18" s="5" t="n">
-        <v>45071.87102304934</v>
+        <v>45072.2939245805</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>45071.87103462341</v>
+        <v>45072.2939245805</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Supplier Y</t>
+          <t>Supplier L</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[{'Name': 'Level', 'Quantity': 200}, {'Name': 'Measuring Tape', 'Quantity': 500}, {'Name': 'Screwdriver Set', 'Quantity': 200}, {'Name': 'Utility Knife', 'Quantity': 200}, {'Name': 'Hammer', 'Quantity': 300}]</t>
+          <t>[{'Name': 'Moisturizing Cream', 'Quantity': 300}]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>50016</v>
+        <v>50014</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -925,19 +925,19 @@
         </is>
       </c>
       <c r="C19" s="5" t="n">
-        <v>45071.87102310723</v>
+        <v>45072.29392459213</v>
       </c>
       <c r="D19" s="5" t="n">
-        <v>45071.87102310723</v>
+        <v>45072.29393616621</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Supplier W</t>
+          <t>Supplier M</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[{'Name': 'Blender', 'Quantity': 100}]</t>
+          <t>[{'Name': 'Mascara', 'Quantity': 500}, {'Name': 'Lipstick', 'Quantity': 500}]</t>
         </is>
       </c>
     </row>
@@ -951,19 +951,19 @@
         </is>
       </c>
       <c r="C20" s="5" t="n">
-        <v>45071.87102312523</v>
+        <v>45072.29392462684</v>
       </c>
       <c r="D20" s="5" t="n">
-        <v>45071.87102312523</v>
+        <v>45072.29393620091</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Supplier T</t>
+          <t>Supplier R</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[{'Name': 'Cookware Set', 'Quantity': 100}]</t>
+          <t>[{'Name': 'Vacuum Cleaner', 'Quantity': 100}]</t>
         </is>
       </c>
     </row>
@@ -977,19 +977,19 @@
         </is>
       </c>
       <c r="C21" s="5" t="n">
-        <v>45071.87102319468</v>
+        <v>45072.29392466156</v>
       </c>
       <c r="D21" s="5" t="n">
-        <v>45071.87102319468</v>
+        <v>45072.29393623563</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Supplier O</t>
+          <t>Supplier C</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[{'Name': 'Bed Sheets', 'Quantity': 200}]</t>
+          <t>[{'Name': 'Bluetooth Speaker', 'Quantity': 200}, {'Name': 'Wireless Mouse', 'Quantity': 200}]</t>
         </is>
       </c>
     </row>

</xml_diff>